<commit_message>
Update visualize(). It fully works now :(
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jackygunter\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jackygunter\Documents\GitHub\production-scheduling\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68B0AC49-0108-45B8-BDDB-D2300A935AC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08A2BC6A-484C-403B-A139-9AA4E6C39AAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -764,8 +764,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Q50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1168,7 +1168,7 @@
         <v>25.999999999999947</v>
       </c>
       <c r="J14" s="15">
-        <f t="shared" ref="J14:L14" si="3">C7</f>
+        <f t="shared" ref="J14" si="3">C7</f>
         <v>0</v>
       </c>
       <c r="K14" s="15">
@@ -1489,7 +1489,7 @@
       </c>
       <c r="P26" s="15"/>
       <c r="Q26" s="15">
-        <f t="shared" ref="O26:Q26" si="15">Q20+Q21</f>
+        <f t="shared" ref="Q26" si="15">Q20+Q21</f>
         <v>1</v>
       </c>
     </row>

</xml_diff>